<commit_message>
saved final results of 500 dim run
</commit_message>
<xml_diff>
--- a/modified_matlab_code+data/Results/Comparison Results, Brynn Cross.xlsx
+++ b/modified_matlab_code+data/Results/Comparison Results, Brynn Cross.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schew\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brycefitzgerald/Documents/GitHub/research_pipeline/modified_matlab_code+data/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB291C73-9F4A-43C9-AC45-69C4E3E7D658}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F7424-64FC-1143-AFD8-D0CA62014AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="311" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10240" yWindow="0" windowWidth="18560" windowHeight="18000" tabRatio="311" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2D" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="86">
   <si>
     <t>d = 2</t>
   </si>
@@ -296,10 +296,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +340,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -385,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,6 +472,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -792,13 +811,13 @@
       <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>82</v>
       </c>
@@ -819,7 +838,7 @@
       <c r="P1" s="25"/>
       <c r="Q1" s="25"/>
     </row>
-    <row r="2" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="2" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -840,7 +859,7 @@
       <c r="P2" s="26"/>
       <c r="Q2" s="26"/>
     </row>
-    <row r="3" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="3" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
@@ -874,7 +893,7 @@
       </c>
       <c r="Q3" s="27"/>
     </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="4" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
@@ -899,7 +918,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="10"/>
     </row>
-    <row r="5" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="5" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>31</v>
       </c>
@@ -952,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="6" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
@@ -977,7 +996,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="10"/>
     </row>
-    <row r="7" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="7" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>34</v>
       </c>
@@ -1030,7 +1049,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="8" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>40</v>
       </c>
@@ -1055,7 +1074,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="9" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>39</v>
       </c>
@@ -1080,7 +1099,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="10" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
@@ -1105,7 +1124,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="11" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>33</v>
       </c>
@@ -1158,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="12" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>35</v>
       </c>
@@ -1211,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="13" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>53</v>
       </c>
@@ -1264,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="14" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
@@ -1289,7 +1308,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="15" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>30</v>
       </c>
@@ -1342,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="16" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>29</v>
       </c>
@@ -1395,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="17" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>41</v>
       </c>
@@ -1448,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="18" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
@@ -1501,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="19" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
@@ -1554,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="20" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>44</v>
       </c>
@@ -1579,7 +1598,7 @@
       <c r="P20" s="9"/>
       <c r="Q20" s="10"/>
     </row>
-    <row r="21" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="21" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>46</v>
       </c>
@@ -1632,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="22" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>38</v>
       </c>
@@ -1685,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="23" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>16</v>
       </c>
@@ -1738,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="24" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>52</v>
       </c>
@@ -1763,7 +1782,7 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="25" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>51</v>
       </c>
@@ -1816,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="26" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>17</v>
       </c>
@@ -1869,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="27" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>28</v>
       </c>
@@ -1922,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="28" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>9</v>
       </c>
@@ -1975,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="29" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>27</v>
       </c>
@@ -2028,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="30" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>48</v>
       </c>
@@ -2053,7 +2072,7 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="31" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>25</v>
       </c>
@@ -2106,7 +2125,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="32" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>11</v>
       </c>
@@ -2131,7 +2150,7 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="11"/>
     </row>
-    <row r="33" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="33" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>45</v>
       </c>
@@ -2156,7 +2175,7 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="34" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>50</v>
       </c>
@@ -2209,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="35" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>36</v>
       </c>
@@ -2234,7 +2253,7 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="36" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>12</v>
       </c>
@@ -2259,7 +2278,7 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="11"/>
     </row>
-    <row r="37" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="37" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>26</v>
       </c>
@@ -2312,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="38" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>13</v>
       </c>
@@ -2337,7 +2356,7 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="11"/>
     </row>
-    <row r="39" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="39" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>49</v>
       </c>
@@ -2362,7 +2381,7 @@
       <c r="P39" s="9"/>
       <c r="Q39" s="10"/>
     </row>
-    <row r="40" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="40" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>21</v>
       </c>
@@ -2387,7 +2406,7 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="11"/>
     </row>
-    <row r="41" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="41" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
@@ -2412,7 +2431,7 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="11"/>
     </row>
-    <row r="42" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="42" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>19</v>
       </c>
@@ -2437,7 +2456,7 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="11"/>
     </row>
-    <row r="43" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="43" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>22</v>
       </c>
@@ -2462,7 +2481,7 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="11"/>
     </row>
-    <row r="44" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="44" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>23</v>
       </c>
@@ -2487,7 +2506,7 @@
       <c r="P44" s="9"/>
       <c r="Q44" s="10"/>
     </row>
-    <row r="45" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="45" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>24</v>
       </c>
@@ -2512,7 +2531,7 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="11"/>
     </row>
-    <row r="46" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="46" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>20</v>
       </c>
@@ -2565,7 +2584,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="47" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>47</v>
       </c>
@@ -2586,7 +2605,7 @@
       <c r="P47" s="9"/>
       <c r="Q47" s="10"/>
     </row>
-    <row r="48" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="48" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="4"/>
       <c r="C48" s="11"/>
@@ -2605,7 +2624,7 @@
       <c r="P48" s="4"/>
       <c r="Q48" s="11"/>
     </row>
-    <row r="49" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="49" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="4"/>
       <c r="C49" s="11"/>
@@ -2624,7 +2643,7 @@
       <c r="P49" s="4"/>
       <c r="Q49" s="11"/>
     </row>
-    <row r="50" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="50" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="4"/>
       <c r="C50" s="11"/>
@@ -2643,7 +2662,7 @@
       <c r="P50" s="4"/>
       <c r="Q50" s="11"/>
     </row>
-    <row r="51" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="51" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="4"/>
       <c r="C51" s="11"/>
@@ -2662,7 +2681,7 @@
       <c r="P51" s="4"/>
       <c r="Q51" s="11"/>
     </row>
-    <row r="52" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="52" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="4"/>
       <c r="C52" s="11"/>
@@ -2681,7 +2700,7 @@
       <c r="P52" s="4"/>
       <c r="Q52" s="11"/>
     </row>
-    <row r="53" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="53" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="4"/>
       <c r="C53" s="11"/>
@@ -2700,7 +2719,7 @@
       <c r="P53" s="4"/>
       <c r="Q53" s="11"/>
     </row>
-    <row r="54" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="54" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="26" t="s">
         <v>1</v>
       </c>
@@ -2721,7 +2740,7 @@
       <c r="P54" s="26"/>
       <c r="Q54" s="26"/>
     </row>
-    <row r="55" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="55" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>10</v>
       </c>
@@ -2744,7 +2763,7 @@
       <c r="N55" s="4"/>
       <c r="O55" s="5"/>
     </row>
-    <row r="56" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="56" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="4"/>
       <c r="C56" s="5"/>
@@ -2761,7 +2780,7 @@
       <c r="N56" s="4"/>
       <c r="O56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="57" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="4"/>
       <c r="C57" s="5"/>
@@ -2778,7 +2797,7 @@
       <c r="N57" s="4"/>
       <c r="O57" s="5"/>
     </row>
-    <row r="58" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="58" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="4"/>
       <c r="C58" s="5"/>
@@ -2795,7 +2814,7 @@
       <c r="N58" s="4"/>
       <c r="O58" s="5"/>
     </row>
-    <row r="59" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="59" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="4"/>
       <c r="C59" s="5"/>
@@ -2812,7 +2831,7 @@
       <c r="N59" s="4"/>
       <c r="O59" s="5"/>
     </row>
-    <row r="60" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="60" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
@@ -2829,7 +2848,7 @@
       <c r="N60" s="4"/>
       <c r="O60" s="5"/>
     </row>
-    <row r="61" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="61" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="4"/>
       <c r="C61" s="5"/>
@@ -2846,7 +2865,7 @@
       <c r="N61" s="4"/>
       <c r="O61" s="5"/>
     </row>
-    <row r="62" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="62" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="4"/>
       <c r="C62" s="5"/>
@@ -2863,7 +2882,7 @@
       <c r="N62" s="4"/>
       <c r="O62" s="5"/>
     </row>
-    <row r="63" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="63" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="4"/>
       <c r="C63" s="5"/>
@@ -2880,7 +2899,7 @@
       <c r="N63" s="4"/>
       <c r="O63" s="5"/>
     </row>
-    <row r="64" spans="1:17" s="3" customFormat="1" ht="15.75">
+    <row r="64" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="4"/>
       <c r="C64" s="5"/>
@@ -2897,7 +2916,7 @@
       <c r="N64" s="4"/>
       <c r="O64" s="5"/>
     </row>
-    <row r="65" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="65" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
@@ -2914,7 +2933,7 @@
       <c r="N65" s="4"/>
       <c r="O65" s="5"/>
     </row>
-    <row r="66" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="66" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
       <c r="B66" s="4"/>
       <c r="C66" s="5"/>
@@ -2931,7 +2950,7 @@
       <c r="N66" s="4"/>
       <c r="O66" s="5"/>
     </row>
-    <row r="67" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="67" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
       <c r="B67" s="4"/>
       <c r="C67" s="5"/>
@@ -2948,7 +2967,7 @@
       <c r="N67" s="4"/>
       <c r="O67" s="5"/>
     </row>
-    <row r="68" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="68" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="6"/>
       <c r="B68" s="4"/>
       <c r="C68" s="5"/>
@@ -2965,7 +2984,7 @@
       <c r="N68" s="4"/>
       <c r="O68" s="5"/>
     </row>
-    <row r="69" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="69" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
       <c r="B69" s="4"/>
       <c r="C69" s="5"/>
@@ -2982,7 +3001,7 @@
       <c r="N69" s="4"/>
       <c r="O69" s="5"/>
     </row>
-    <row r="70" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="70" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
       <c r="B70" s="4"/>
       <c r="C70" s="5"/>
@@ -2999,7 +3018,7 @@
       <c r="N70" s="4"/>
       <c r="O70" s="5"/>
     </row>
-    <row r="71" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="71" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
       <c r="B71" s="4"/>
       <c r="C71" s="5"/>
@@ -3016,7 +3035,7 @@
       <c r="N71" s="4"/>
       <c r="O71" s="5"/>
     </row>
-    <row r="72" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="72" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="6"/>
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
@@ -3033,7 +3052,7 @@
       <c r="N72" s="4"/>
       <c r="O72" s="5"/>
     </row>
-    <row r="73" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="73" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="6"/>
       <c r="B73" s="4"/>
       <c r="C73" s="5"/>
@@ -3050,7 +3069,7 @@
       <c r="N73" s="4"/>
       <c r="O73" s="5"/>
     </row>
-    <row r="74" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="74" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="6"/>
       <c r="B74" s="4"/>
       <c r="C74" s="5"/>
@@ -3067,7 +3086,7 @@
       <c r="N74" s="4"/>
       <c r="O74" s="5"/>
     </row>
-    <row r="75" spans="1:15" s="3" customFormat="1" ht="15.75">
+    <row r="75" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
       <c r="B75" s="4"/>
       <c r="C75" s="5"/>
@@ -3084,7 +3103,7 @@
       <c r="N75" s="4"/>
       <c r="O75" s="5"/>
     </row>
-    <row r="76" spans="1:15" ht="15.75">
+    <row r="76" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="6"/>
       <c r="B76" s="4"/>
       <c r="C76" s="5"/>
@@ -3101,7 +3120,7 @@
       <c r="N76" s="4"/>
       <c r="O76" s="5"/>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="C77" s="1"/>
       <c r="E77" s="1"/>
@@ -3112,7 +3131,7 @@
       <c r="O77" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A4:O47">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:O47">
     <sortCondition ref="B4:B47"/>
   </sortState>
   <mergeCells count="11">
@@ -3142,28 +3161,28 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.5" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" customWidth="1"/>
+    <col min="20" max="20" width="9.5" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" customHeight="1">
+    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>70</v>
       </c>
@@ -3188,7 +3207,7 @@
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
     </row>
-    <row r="2" spans="1:21" ht="18.75" customHeight="1">
+    <row r="2" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -3231,7 +3250,7 @@
       </c>
       <c r="U2" s="28"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -3292,7 +3311,7 @@
         <v>29269</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75">
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -3353,7 +3372,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75">
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -3414,7 +3433,7 @@
         <v>60429</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -3475,7 +3494,7 @@
         <v>31042</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75">
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -3536,7 +3555,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75">
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
@@ -3597,7 +3616,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75">
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -3658,7 +3677,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75">
+    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -3719,7 +3738,7 @@
         <v>23076</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75">
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>62</v>
       </c>
@@ -3780,7 +3799,7 @@
         <v>26199</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75">
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
@@ -3841,7 +3860,7 @@
         <v>35950</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75">
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>64</v>
       </c>
@@ -3902,7 +3921,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75">
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>71</v>
       </c>
@@ -3963,7 +3982,7 @@
         <v>56267</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75">
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>72</v>
       </c>
@@ -4024,7 +4043,7 @@
         <v>63117</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75">
+    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>73</v>
       </c>
@@ -4085,7 +4104,7 @@
         <v>32990</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75">
+    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
@@ -4146,7 +4165,7 @@
         <v>32917</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75">
+    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -4170,7 +4189,7 @@
       <c r="O18" s="15"/>
       <c r="P18" s="23"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75">
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>80</v>
       </c>
@@ -4193,7 +4212,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="15.75">
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>77</v>
       </c>
@@ -4216,7 +4235,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:21" ht="15.75">
+    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>78</v>
       </c>
@@ -4239,7 +4258,7 @@
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>79</v>
       </c>
@@ -4262,7 +4281,7 @@
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75">
+    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -4279,7 +4298,7 @@
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75">
+    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -4296,7 +4315,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75">
+    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -4313,7 +4332,7 @@
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -4330,7 +4349,7 @@
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75">
+    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -4347,7 +4366,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75">
+    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -4364,7 +4383,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -4381,7 +4400,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75">
+    <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -4398,7 +4417,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75">
+    <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -4415,7 +4434,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75">
+    <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -4432,7 +4451,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -4449,7 +4468,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -4466,7 +4485,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -4483,7 +4502,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -4500,7 +4519,7 @@
       <c r="N36" s="14"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -4517,7 +4536,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -4534,7 +4553,7 @@
       <c r="N38" s="14"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75">
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -4551,7 +4570,7 @@
       <c r="N39" s="14"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75">
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -4568,7 +4587,7 @@
       <c r="N40" s="14"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75">
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -4585,7 +4604,7 @@
       <c r="N41" s="14"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -4602,7 +4621,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75">
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -4619,7 +4638,7 @@
       <c r="N43" s="14"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -4636,7 +4655,7 @@
       <c r="N44" s="14"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -4653,7 +4672,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75">
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -4698,27 +4717,27 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.5" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" customWidth="1"/>
+    <col min="20" max="20" width="10.1640625" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" customHeight="1">
+    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>69</v>
       </c>
@@ -4743,7 +4762,7 @@
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
     </row>
-    <row r="2" spans="1:21" ht="17.25" customHeight="1">
+    <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -4786,7 +4805,7 @@
       </c>
       <c r="U2" s="29"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -4847,7 +4866,7 @@
         <v>106330</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75">
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -4908,7 +4927,7 @@
         <v>88410</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75">
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -4969,7 +4988,7 @@
         <v>191676</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -5030,7 +5049,7 @@
         <v>115245</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75">
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -5091,7 +5110,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75">
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
@@ -5152,7 +5171,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75">
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -5213,7 +5232,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75">
+    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -5274,7 +5293,7 @@
         <v>81475</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75">
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>62</v>
       </c>
@@ -5335,7 +5354,7 @@
         <v>95415</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75">
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
@@ -5396,7 +5415,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75">
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>64</v>
       </c>
@@ -5457,7 +5476,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75">
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>71</v>
       </c>
@@ -5518,7 +5537,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75">
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>72</v>
       </c>
@@ -5579,7 +5598,7 @@
         <v>215110</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75">
+    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>73</v>
       </c>
@@ -5640,7 +5659,7 @@
         <v>124378</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75">
+    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
@@ -5701,7 +5720,7 @@
         <v>124435</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75">
+    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -5724,7 +5743,7 @@
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75">
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>80</v>
       </c>
@@ -5747,7 +5766,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="15.75">
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>77</v>
       </c>
@@ -5770,7 +5789,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:21" ht="15.75">
+    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>78</v>
       </c>
@@ -5793,7 +5812,7 @@
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>79</v>
       </c>
@@ -5816,7 +5835,7 @@
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75">
+    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -5833,7 +5852,7 @@
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75">
+    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -5850,7 +5869,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75">
+    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -5867,7 +5886,7 @@
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -5884,7 +5903,7 @@
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75">
+    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -5901,7 +5920,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75">
+    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -5918,7 +5937,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -5935,7 +5954,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75">
+    <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -5952,7 +5971,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75">
+    <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -5969,7 +5988,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75">
+    <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -5986,7 +6005,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -6003,7 +6022,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -6020,7 +6039,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -6037,7 +6056,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -6054,7 +6073,7 @@
       <c r="N36" s="14"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -6071,7 +6090,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -6088,7 +6107,7 @@
       <c r="N38" s="14"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75">
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -6105,7 +6124,7 @@
       <c r="N39" s="14"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75">
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -6122,7 +6141,7 @@
       <c r="N40" s="14"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75">
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -6139,7 +6158,7 @@
       <c r="N41" s="14"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -6156,7 +6175,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75">
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -6173,7 +6192,7 @@
       <c r="N43" s="14"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -6190,7 +6209,7 @@
       <c r="N44" s="14"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -6207,7 +6226,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75">
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -6251,25 +6270,25 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" customWidth="1"/>
+    <col min="13" max="13" width="10.5" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" customWidth="1"/>
+    <col min="18" max="18" width="12.5" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
     <col min="20" max="21" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.75" customHeight="1">
+    <row r="1" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>68</v>
       </c>
@@ -6294,7 +6313,7 @@
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
     </row>
-    <row r="2" spans="1:21" ht="18" customHeight="1">
+    <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -6337,7 +6356,7 @@
       </c>
       <c r="U2" s="28"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -6398,7 +6417,7 @@
         <v>190687</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75">
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -6459,7 +6478,7 @@
         <v>156578</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75">
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -6520,7 +6539,7 @@
         <v>327153</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -6581,7 +6600,7 @@
         <v>209277</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75">
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -6642,7 +6661,7 @@
         <v>499000</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75">
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
@@ -6703,7 +6722,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75">
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -6764,7 +6783,7 @@
         <v>23219</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75">
+    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -6825,7 +6844,7 @@
         <v>150360</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75">
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>62</v>
       </c>
@@ -6886,7 +6905,7 @@
         <v>173028</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75">
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
@@ -6947,7 +6966,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75">
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>64</v>
       </c>
@@ -7008,7 +7027,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75">
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>71</v>
       </c>
@@ -7069,7 +7088,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75">
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>72</v>
       </c>
@@ -7130,7 +7149,7 @@
         <v>377617</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75">
+    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>73</v>
       </c>
@@ -7191,7 +7210,7 @@
         <v>229480</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75">
+    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
@@ -7252,7 +7271,7 @@
         <v>229604</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75">
+    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -7275,7 +7294,7 @@
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75">
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>80</v>
       </c>
@@ -7298,7 +7317,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="15.75">
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>77</v>
       </c>
@@ -7321,7 +7340,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:21" ht="15.75">
+    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>78</v>
       </c>
@@ -7344,7 +7363,7 @@
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>79</v>
       </c>
@@ -7367,7 +7386,7 @@
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75">
+    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -7384,7 +7403,7 @@
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75">
+    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -7401,7 +7420,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75">
+    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -7418,7 +7437,7 @@
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -7435,7 +7454,7 @@
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75">
+    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -7452,7 +7471,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75">
+    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -7469,7 +7488,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -7486,7 +7505,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75">
+    <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -7503,7 +7522,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75">
+    <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -7520,7 +7539,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75">
+    <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -7537,7 +7556,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -7554,7 +7573,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -7571,7 +7590,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -7588,7 +7607,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -7605,7 +7624,7 @@
       <c r="N36" s="14"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -7622,7 +7641,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -7639,7 +7658,7 @@
       <c r="N38" s="14"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75">
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -7656,7 +7675,7 @@
       <c r="N39" s="14"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75">
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -7673,7 +7692,7 @@
       <c r="N40" s="14"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75">
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -7690,7 +7709,7 @@
       <c r="N41" s="14"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -7707,7 +7726,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75">
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -7724,7 +7743,7 @@
       <c r="N43" s="14"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -7741,7 +7760,7 @@
       <c r="N44" s="14"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -7758,7 +7777,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75">
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -7803,28 +7822,28 @@
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.5" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" customHeight="1">
+    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>67</v>
       </c>
@@ -7849,7 +7868,7 @@
       <c r="T1" s="30"/>
       <c r="U1" s="30"/>
     </row>
-    <row r="2" spans="1:21" ht="18.75" customHeight="1">
+    <row r="2" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -7892,7 +7911,7 @@
       </c>
       <c r="U2" s="28"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -7957,7 +7976,7 @@
         <v>419507</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75">
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -8022,7 +8041,7 @@
         <v>343334</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75">
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -8087,7 +8106,7 @@
         <v>678848</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -8152,7 +8171,7 @@
         <v>473714</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75">
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -8217,7 +8236,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75">
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
@@ -8282,7 +8301,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75">
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -8347,7 +8366,7 @@
         <v>97000</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75">
+    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -8412,7 +8431,7 @@
         <v>645875</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75">
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>62</v>
       </c>
@@ -8477,7 +8496,7 @@
         <v>381944</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75">
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
@@ -8542,7 +8561,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75">
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>64</v>
       </c>
@@ -8607,7 +8626,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75">
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>71</v>
       </c>
@@ -8672,7 +8691,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75">
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>72</v>
       </c>
@@ -8737,7 +8756,7 @@
         <v>810825</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75">
+    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>73</v>
       </c>
@@ -8802,7 +8821,7 @@
         <v>522540</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75">
+    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
@@ -8867,7 +8886,7 @@
         <v>521394</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75">
+    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -8890,7 +8909,7 @@
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75">
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>80</v>
       </c>
@@ -8913,7 +8932,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="15.75">
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>77</v>
       </c>
@@ -8936,7 +8955,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:21" ht="15.75">
+    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>78</v>
       </c>
@@ -8959,7 +8978,7 @@
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>79</v>
       </c>
@@ -8982,7 +9001,7 @@
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75">
+    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -8999,7 +9018,7 @@
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75">
+    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -9016,7 +9035,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75">
+    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -9033,7 +9052,7 @@
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -9050,7 +9069,7 @@
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75">
+    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -9067,7 +9086,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75">
+    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -9084,7 +9103,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -9101,7 +9120,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75">
+    <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -9118,7 +9137,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75">
+    <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -9135,7 +9154,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75">
+    <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -9152,7 +9171,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -9169,7 +9188,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -9186,7 +9205,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -9203,7 +9222,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -9220,7 +9239,7 @@
       <c r="N36" s="14"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -9237,7 +9256,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -9254,7 +9273,7 @@
       <c r="N38" s="14"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75">
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -9271,7 +9290,7 @@
       <c r="N39" s="14"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75">
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -9288,7 +9307,7 @@
       <c r="N40" s="14"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75">
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -9305,7 +9324,7 @@
       <c r="N41" s="14"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -9322,7 +9341,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75">
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -9339,7 +9358,7 @@
       <c r="N43" s="14"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -9356,7 +9375,7 @@
       <c r="N44" s="14"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -9373,7 +9392,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75">
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -9392,6 +9411,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -9400,12 +9425,6 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9421,30 +9440,30 @@
       <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="4.83203125" customWidth="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="20" width="10.85546875" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="18" max="20" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" customHeight="1">
+    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>66</v>
       </c>
@@ -9469,7 +9488,7 @@
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
     </row>
-    <row r="2" spans="1:21" ht="17.25" customHeight="1">
+    <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -9512,7 +9531,7 @@
       </c>
       <c r="U2" s="28"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -9577,7 +9596,7 @@
         <v>2333100</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75">
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -9642,7 +9661,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75">
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -9707,7 +9726,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -9772,7 +9791,7 @@
         <v>2709300</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75">
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -9837,7 +9856,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75">
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
@@ -9902,7 +9921,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75">
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -9967,7 +9986,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75">
+    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -10032,7 +10051,7 @@
         <v>3155175</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75">
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>62</v>
       </c>
@@ -10097,7 +10116,7 @@
         <v>3446721</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75">
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
@@ -10162,7 +10181,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75">
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>64</v>
       </c>
@@ -10227,7 +10246,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75">
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>71</v>
       </c>
@@ -10292,7 +10311,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75">
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>72</v>
       </c>
@@ -10357,7 +10376,7 @@
         <v>4569075</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75">
+    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>73</v>
       </c>
@@ -10418,7 +10437,7 @@
       <c r="T16" s="4"/>
       <c r="U16" s="5"/>
     </row>
-    <row r="17" spans="1:21" ht="15.75">
+    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
@@ -10479,7 +10498,7 @@
       <c r="T17" s="4"/>
       <c r="U17" s="5"/>
     </row>
-    <row r="18" spans="1:21" ht="15.75">
+    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -10502,7 +10521,7 @@
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75">
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>80</v>
       </c>
@@ -10525,7 +10544,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="15.75">
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>77</v>
       </c>
@@ -10548,7 +10567,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:21" ht="15.75">
+    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>78</v>
       </c>
@@ -10571,7 +10590,7 @@
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>79</v>
       </c>
@@ -10594,7 +10613,7 @@
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75">
+    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -10611,7 +10630,7 @@
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75">
+    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -10628,7 +10647,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75">
+    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -10645,7 +10664,7 @@
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -10662,7 +10681,7 @@
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75">
+    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -10679,7 +10698,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75">
+    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -10696,7 +10715,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -10713,7 +10732,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75">
+    <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -10730,7 +10749,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75">
+    <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -10747,7 +10766,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75">
+    <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -10764,7 +10783,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -10781,7 +10800,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -10798,7 +10817,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -10815,7 +10834,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -10832,7 +10851,7 @@
       <c r="N36" s="14"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -10849,7 +10868,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -10866,7 +10885,7 @@
       <c r="N38" s="14"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75">
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -10883,7 +10902,7 @@
       <c r="N39" s="14"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75">
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -10900,7 +10919,7 @@
       <c r="N40" s="14"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75">
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -10917,7 +10936,7 @@
       <c r="N41" s="14"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -10934,7 +10953,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75">
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -10951,7 +10970,7 @@
       <c r="N43" s="14"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -10968,7 +10987,7 @@
       <c r="N44" s="14"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -10985,7 +11004,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75">
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -11026,33 +11045,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="7" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
+    <col min="11" max="11" width="5.5" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" customWidth="1"/>
-    <col min="17" max="18" width="11.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" customWidth="1"/>
+    <col min="15" max="15" width="4.5" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
+    <col min="17" max="18" width="11.33203125" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="20.25" customHeight="1">
+    <row r="1" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>65</v>
       </c>
@@ -11077,7 +11096,7 @@
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
     </row>
-    <row r="2" spans="1:21" ht="17.25" customHeight="1">
+    <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -11120,7 +11139,7 @@
       </c>
       <c r="U2" s="28"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -11178,8 +11197,14 @@
       <c r="S3" s="11">
         <v>22680</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75">
+      <c r="T3" s="31">
+        <v>1</v>
+      </c>
+      <c r="U3" s="34">
+        <v>4902560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -11237,8 +11262,14 @@
       <c r="S4" s="11">
         <v>32600</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75">
+      <c r="T4" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="U4" s="34">
+        <v>3895200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -11296,8 +11327,14 @@
       <c r="S5" s="11">
         <v>101600</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75">
+      <c r="T5" s="32">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -11355,8 +11392,14 @@
       <c r="S6" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75">
+      <c r="T6" s="32">
+        <v>1</v>
+      </c>
+      <c r="U6" s="34">
+        <v>5824080</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -11414,8 +11457,14 @@
       <c r="S7" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75">
+      <c r="T7" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="U7" s="34">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
@@ -11473,8 +11522,14 @@
       <c r="S8" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75">
+      <c r="T8" s="32">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -11532,8 +11587,14 @@
       <c r="S9" s="11">
         <v>15080</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75">
+      <c r="T9" s="32">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -11591,8 +11652,14 @@
       <c r="S10" s="11">
         <v>2930280</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75">
+      <c r="T10" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="U10" s="34">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>62</v>
       </c>
@@ -11646,8 +11713,14 @@
       <c r="S11" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75">
+      <c r="T11" s="32">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
@@ -11701,8 +11774,14 @@
       <c r="S12" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75">
+      <c r="T12" s="32">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>64</v>
       </c>
@@ -11756,8 +11835,14 @@
       <c r="S13" s="11">
         <v>38360</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75">
+      <c r="T13" s="32">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>71</v>
       </c>
@@ -11811,8 +11896,14 @@
       <c r="S14" s="11">
         <v>74920</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75">
+      <c r="T14" s="32">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>72</v>
       </c>
@@ -11870,8 +11961,14 @@
       <c r="S15" s="11">
         <v>139560</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75">
+      <c r="T15" s="31">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>73</v>
       </c>
@@ -11929,8 +12026,14 @@
       <c r="S16" s="11">
         <v>63800</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75">
+      <c r="T16" s="33">
+        <v>1</v>
+      </c>
+      <c r="U16" s="34">
+        <v>646040</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
@@ -11988,8 +12091,14 @@
       <c r="S17" s="11">
         <v>40600</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.75">
+      <c r="T17" s="31">
+        <v>1</v>
+      </c>
+      <c r="U17" s="34">
+        <v>634360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -12012,7 +12121,7 @@
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75">
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>80</v>
       </c>
@@ -12035,7 +12144,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75">
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>77</v>
       </c>
@@ -12058,7 +12167,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:19" ht="15.75">
+    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>78</v>
       </c>
@@ -12081,7 +12190,7 @@
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:19" ht="15.75">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>79</v>
       </c>
@@ -12104,7 +12213,7 @@
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
     </row>
-    <row r="23" spans="1:19" ht="15.75">
+    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -12121,7 +12230,7 @@
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75">
+    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -12138,7 +12247,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
     </row>
-    <row r="25" spans="1:19" ht="15.75">
+    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -12155,7 +12264,7 @@
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:19" ht="15.75">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -12172,7 +12281,7 @@
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:19" ht="15.75">
+    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -12189,7 +12298,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:19" ht="15.75">
+    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -12206,7 +12315,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:19" ht="15.75">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -12223,7 +12332,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:19" ht="15.75">
+    <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -12240,7 +12349,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:19" ht="15.75">
+    <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -12257,7 +12366,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:19" ht="15.75">
+    <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -12274,7 +12383,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -12291,7 +12400,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -12308,7 +12417,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -12325,7 +12434,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -12342,7 +12451,7 @@
       <c r="N36" s="14"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -12359,7 +12468,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -12376,7 +12485,7 @@
       <c r="N38" s="14"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75">
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -12393,7 +12502,7 @@
       <c r="N39" s="14"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75">
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -12410,7 +12519,7 @@
       <c r="N40" s="14"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75">
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -12427,7 +12536,7 @@
       <c r="N41" s="14"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -12444,7 +12553,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75">
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -12461,7 +12570,7 @@
       <c r="N43" s="14"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -12478,7 +12587,7 @@
       <c r="N44" s="14"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -12495,7 +12604,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75">
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -12540,32 +12649,32 @@
       <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="5.5" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" customWidth="1"/>
+    <col min="17" max="17" width="13.5" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="22.5" customHeight="1">
+    <row r="1" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>75</v>
       </c>
@@ -12590,7 +12699,7 @@
       <c r="T1" s="21"/>
       <c r="U1" s="21"/>
     </row>
-    <row r="2" spans="1:21" ht="18" customHeight="1">
+    <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="29" t="s">
         <v>2</v>
@@ -12633,7 +12742,7 @@
       </c>
       <c r="U2" s="28"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -12692,7 +12801,7 @@
         <v>26650</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75">
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -12751,7 +12860,7 @@
         <v>38500</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75">
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -12810,7 +12919,7 @@
         <v>106850</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75">
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>57</v>
       </c>
@@ -12869,7 +12978,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75">
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>58</v>
       </c>
@@ -12928,7 +13037,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75">
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>59</v>
       </c>
@@ -12987,7 +13096,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75">
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>60</v>
       </c>
@@ -13046,7 +13155,7 @@
         <v>21450</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75">
+    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>61</v>
       </c>
@@ -13105,7 +13214,7 @@
         <v>7383800</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75">
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>62</v>
       </c>
@@ -13164,7 +13273,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75">
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
@@ -13223,7 +13332,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75">
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>64</v>
       </c>
@@ -13278,7 +13387,7 @@
         <v>42400</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75">
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>71</v>
       </c>
@@ -13333,7 +13442,7 @@
         <v>92900</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75">
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>72</v>
       </c>
@@ -13392,7 +13501,7 @@
         <v>175150</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75">
+    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>73</v>
       </c>
@@ -13451,7 +13560,7 @@
         <v>77700</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75">
+    <row r="17" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>74</v>
       </c>
@@ -13510,7 +13619,7 @@
         <v>48200</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75">
+    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -13533,7 +13642,7 @@
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75">
+    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>80</v>
       </c>
@@ -13552,7 +13661,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75">
+    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>77</v>
       </c>
@@ -13575,7 +13684,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
     </row>
-    <row r="21" spans="1:19" ht="15.75">
+    <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>78</v>
       </c>
@@ -13598,7 +13707,7 @@
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
     </row>
-    <row r="22" spans="1:19" ht="15.75">
+    <row r="22" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>79</v>
       </c>
@@ -13621,7 +13730,7 @@
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
     </row>
-    <row r="23" spans="1:19" ht="15.75">
+    <row r="23" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -13638,7 +13747,7 @@
       <c r="N23" s="14"/>
       <c r="O23" s="15"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75">
+    <row r="24" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -13655,7 +13764,7 @@
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
     </row>
-    <row r="25" spans="1:19" ht="15.75">
+    <row r="25" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -13672,7 +13781,7 @@
       <c r="N25" s="14"/>
       <c r="O25" s="15"/>
     </row>
-    <row r="26" spans="1:19" ht="15.75">
+    <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -13689,7 +13798,7 @@
       <c r="N26" s="14"/>
       <c r="O26" s="15"/>
     </row>
-    <row r="27" spans="1:19" ht="15.75">
+    <row r="27" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -13706,7 +13815,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
     </row>
-    <row r="28" spans="1:19" ht="15.75">
+    <row r="28" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -13723,7 +13832,7 @@
       <c r="N28" s="14"/>
       <c r="O28" s="15"/>
     </row>
-    <row r="29" spans="1:19" ht="15.75">
+    <row r="29" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -13740,7 +13849,7 @@
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:19" ht="15.75">
+    <row r="30" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -13757,7 +13866,7 @@
       <c r="N30" s="14"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:19" ht="15.75">
+    <row r="31" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -13774,7 +13883,7 @@
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:19" ht="15.75">
+    <row r="32" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -13791,7 +13900,7 @@
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75">
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -13808,7 +13917,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75">
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -13825,7 +13934,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="15"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75">
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -13842,7 +13951,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="15"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75">
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -13859,7 +13968,7 @@
       <c r="N36" s="14"/>
       <c r="O36" s="15"/>
     </row>
-    <row r="37" spans="1:15" ht="15.75">
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -13876,7 +13985,7 @@
       <c r="N37" s="14"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:15" ht="15.75">
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -13893,7 +14002,7 @@
       <c r="N38" s="14"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:15" ht="15.75">
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -13910,7 +14019,7 @@
       <c r="N39" s="14"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15" ht="15.75">
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -13927,7 +14036,7 @@
       <c r="N40" s="14"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15" ht="15.75">
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -13944,7 +14053,7 @@
       <c r="N41" s="14"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="15.75">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -13961,7 +14070,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15.75">
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -13978,7 +14087,7 @@
       <c r="N43" s="14"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15" ht="15.75">
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -13995,7 +14104,7 @@
       <c r="N44" s="14"/>
       <c r="O44" s="15"/>
     </row>
-    <row r="45" spans="1:15" ht="15.75">
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -14012,7 +14121,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:15" ht="15.75">
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -14031,17 +14140,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test Function 2 @ 1000D Finished
Updated Results in spreadsheet
</commit_message>
<xml_diff>
--- a/modified_matlab_code+data/Results/Comparison Results, Brynn Cross.xlsx
+++ b/modified_matlab_code+data/Results/Comparison Results, Brynn Cross.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brycefitzgerald/Documents/GitHub/research_pipeline/modified_matlab_code+data/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F7424-64FC-1143-AFD8-D0CA62014AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB024CFB-2FA8-3543-BC11-C02CD234E655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="0" windowWidth="18560" windowHeight="18000" tabRatio="311" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10240" yWindow="500" windowWidth="18560" windowHeight="17500" tabRatio="311" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2D" sheetId="1" r:id="rId1"/>
@@ -298,7 +298,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -456,6 +456,18 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,18 +484,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -818,80 +818,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
+      <c r="A2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
     </row>
     <row r="3" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27" t="s">
+      <c r="M3" s="31"/>
+      <c r="N3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27" t="s">
+      <c r="O3" s="31"/>
+      <c r="P3" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="27"/>
+      <c r="Q3" s="31"/>
     </row>
     <row r="4" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -2720,25 +2720,25 @@
       <c r="Q53" s="11"/>
     </row>
     <row r="54" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="26"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="26"/>
-      <c r="N54" s="26"/>
-      <c r="O54" s="26"/>
-      <c r="P54" s="26"/>
-      <c r="Q54" s="26"/>
+      <c r="A54" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="30"/>
+      <c r="K54" s="30"/>
+      <c r="L54" s="30"/>
+      <c r="M54" s="30"/>
+      <c r="N54" s="30"/>
+      <c r="O54" s="30"/>
+      <c r="P54" s="30"/>
+      <c r="Q54" s="30"/>
     </row>
     <row r="55" spans="1:17" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
@@ -3183,23 +3183,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
@@ -3209,46 +3209,46 @@
     </row>
     <row r="2" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="28"/>
+      <c r="U2" s="32"/>
     </row>
     <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -4738,23 +4738,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
@@ -4764,46 +4764,46 @@
     </row>
     <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29" t="s">
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29" t="s">
+      <c r="S2" s="33"/>
+      <c r="T2" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="29"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -6289,23 +6289,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
@@ -6315,46 +6315,46 @@
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="28"/>
+      <c r="U2" s="32"/>
     </row>
     <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -7844,72 +7844,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
     </row>
     <row r="2" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="28"/>
+      <c r="U2" s="32"/>
     </row>
     <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -9411,12 +9411,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -9425,6 +9419,12 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9464,23 +9464,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
@@ -9490,46 +9490,46 @@
     </row>
     <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="28"/>
+      <c r="U2" s="32"/>
     </row>
     <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -11045,7 +11045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -11072,23 +11072,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
@@ -11098,46 +11098,46 @@
     </row>
     <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="28"/>
+      <c r="U2" s="32"/>
     </row>
     <row r="3" spans="1:21" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -11197,10 +11197,10 @@
       <c r="S3" s="11">
         <v>22680</v>
       </c>
-      <c r="T3" s="31">
-        <v>1</v>
-      </c>
-      <c r="U3" s="34">
+      <c r="T3" s="25">
+        <v>1</v>
+      </c>
+      <c r="U3" s="28">
         <v>4902560</v>
       </c>
     </row>
@@ -11262,10 +11262,10 @@
       <c r="S4" s="11">
         <v>32600</v>
       </c>
-      <c r="T4" s="31">
+      <c r="T4" s="25">
         <v>0.1</v>
       </c>
-      <c r="U4" s="34">
+      <c r="U4" s="28">
         <v>3895200</v>
       </c>
     </row>
@@ -11327,7 +11327,7 @@
       <c r="S5" s="11">
         <v>101600</v>
       </c>
-      <c r="T5" s="32">
+      <c r="T5" s="26">
         <v>0</v>
       </c>
       <c r="U5" s="1" t="s">
@@ -11392,10 +11392,10 @@
       <c r="S6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T6" s="32">
-        <v>1</v>
-      </c>
-      <c r="U6" s="34">
+      <c r="T6" s="26">
+        <v>1</v>
+      </c>
+      <c r="U6" s="28">
         <v>5824080</v>
       </c>
     </row>
@@ -11457,10 +11457,10 @@
       <c r="S7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T7" s="32">
+      <c r="T7" s="26">
         <v>0.2</v>
       </c>
-      <c r="U7" s="34">
+      <c r="U7" s="28">
         <v>5000000</v>
       </c>
     </row>
@@ -11522,7 +11522,7 @@
       <c r="S8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T8" s="32">
+      <c r="T8" s="26">
         <v>0</v>
       </c>
       <c r="U8" s="1" t="s">
@@ -11587,7 +11587,7 @@
       <c r="S9" s="11">
         <v>15080</v>
       </c>
-      <c r="T9" s="32">
+      <c r="T9" s="26">
         <v>0</v>
       </c>
       <c r="U9" s="1" t="s">
@@ -11652,10 +11652,10 @@
       <c r="S10" s="11">
         <v>2930280</v>
       </c>
-      <c r="T10" s="31">
+      <c r="T10" s="25">
         <v>0.1</v>
       </c>
-      <c r="U10" s="34">
+      <c r="U10" s="28">
         <v>10000000</v>
       </c>
     </row>
@@ -11713,7 +11713,7 @@
       <c r="S11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T11" s="32">
+      <c r="T11" s="26">
         <v>0</v>
       </c>
       <c r="U11" s="1" t="s">
@@ -11774,7 +11774,7 @@
       <c r="S12" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T12" s="32">
+      <c r="T12" s="26">
         <v>0</v>
       </c>
       <c r="U12" s="1" t="s">
@@ -11835,7 +11835,7 @@
       <c r="S13" s="11">
         <v>38360</v>
       </c>
-      <c r="T13" s="32">
+      <c r="T13" s="26">
         <v>0</v>
       </c>
       <c r="U13" s="1" t="s">
@@ -11896,7 +11896,7 @@
       <c r="S14" s="11">
         <v>74920</v>
       </c>
-      <c r="T14" s="32">
+      <c r="T14" s="26">
         <v>0</v>
       </c>
       <c r="U14" s="1" t="s">
@@ -11961,7 +11961,7 @@
       <c r="S15" s="11">
         <v>139560</v>
       </c>
-      <c r="T15" s="31">
+      <c r="T15" s="25">
         <v>0</v>
       </c>
       <c r="U15" s="1" t="s">
@@ -12026,10 +12026,10 @@
       <c r="S16" s="11">
         <v>63800</v>
       </c>
-      <c r="T16" s="33">
-        <v>1</v>
-      </c>
-      <c r="U16" s="34">
+      <c r="T16" s="27">
+        <v>1</v>
+      </c>
+      <c r="U16" s="28">
         <v>646040</v>
       </c>
     </row>
@@ -12091,10 +12091,10 @@
       <c r="S17" s="11">
         <v>40600</v>
       </c>
-      <c r="T17" s="31">
-        <v>1</v>
-      </c>
-      <c r="U17" s="34">
+      <c r="T17" s="25">
+        <v>1</v>
+      </c>
+      <c r="U17" s="28">
         <v>634360</v>
       </c>
     </row>
@@ -12645,8 +12645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12675,23 +12675,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
@@ -12701,46 +12701,46 @@
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="28"/>
+      <c r="U2" s="32"/>
     </row>
     <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -12799,6 +12799,12 @@
       </c>
       <c r="S3" s="11">
         <v>26650</v>
+      </c>
+      <c r="T3" s="4">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1552950</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
@@ -14140,17 +14146,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>